<commit_message>
Fixed Collision of powerups, tapping functionality
Gun functionality left
</commit_message>
<xml_diff>
--- a/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
+++ b/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Projects\2D-Mobile-Game\2D Mobile Game-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E724F0-14F0-4C25-9154-D1AD6CE81A03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CADEF4-F8D1-419F-89FE-60E9C49DEF8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>Requirements</t>
   </si>
@@ -194,10 +194,7 @@
     <t>WORK IN PROGRESS</t>
   </si>
   <si>
-    <t>Tap for gunshot left</t>
-  </si>
-  <si>
-    <t>Collision of player with powerups not working, need to fix. Put shield in coroutine and create the code for gun pickup. Health is done</t>
+    <t>Create the code for gun pickup</t>
   </si>
 </sst>
 </file>
@@ -318,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -388,6 +385,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -396,23 +411,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,35 +939,35 @@
       </c>
       <c r="D17" s="5">
         <f>SUM(D18:D20)</f>
-        <v>3.5</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5">
-        <v>1</v>
-      </c>
-      <c r="E18" s="37"/>
-    </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
+      <c r="C18" s="40">
+        <v>1</v>
+      </c>
+      <c r="D18" s="40">
+        <v>1</v>
+      </c>
+      <c r="E18" s="31"/>
+    </row>
+    <row r="19" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="5">
-        <v>2</v>
-      </c>
-      <c r="D19" s="5">
-        <v>2</v>
-      </c>
-      <c r="E19" s="37"/>
+      <c r="C19" s="40">
+        <v>2</v>
+      </c>
+      <c r="D19" s="40">
+        <v>1</v>
+      </c>
+      <c r="E19" s="31"/>
     </row>
     <row r="20" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
@@ -976,9 +977,9 @@
         <v>2</v>
       </c>
       <c r="D20" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="38"/>
+        <v>2</v>
+      </c>
+      <c r="E20" s="32"/>
     </row>
     <row r="21" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
@@ -1086,55 +1087,57 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
+    <row r="29" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="23">
         <f>SUM(C30:C32)</f>
-        <v>4</v>
-      </c>
-      <c r="D29" s="16">
+        <v>3</v>
+      </c>
+      <c r="D29" s="23">
         <f>SUM(D30:D32)</f>
-        <v>2</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="17" t="s">
+        <v>2.5</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="18">
-        <v>1</v>
-      </c>
-      <c r="D30" s="18">
-        <v>1</v>
-      </c>
-      <c r="E30" s="31"/>
-    </row>
-    <row r="31" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="17" t="s">
+      <c r="C30" s="8">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
+      <c r="E30" s="28"/>
+    </row>
+    <row r="31" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="18">
-        <v>1</v>
-      </c>
-      <c r="D31" s="18">
-        <v>1</v>
-      </c>
-      <c r="E31" s="31"/>
-    </row>
-    <row r="32" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="13" t="s">
+      <c r="C31" s="8">
+        <v>1</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="E31" s="28"/>
+    </row>
+    <row r="32" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="14">
-        <v>2</v>
-      </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="32"/>
+      <c r="C32" s="10">
+        <v>1</v>
+      </c>
+      <c r="D32" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E32" s="29"/>
     </row>
     <row r="33" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
@@ -1176,7 +1179,7 @@
         <f>SUM(D36:D37)</f>
         <v>0</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="36" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1188,7 +1191,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="18"/>
-      <c r="E36" s="31"/>
+      <c r="E36" s="37"/>
     </row>
     <row r="37" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="13" t="s">
@@ -1198,7 +1201,7 @@
         <v>2</v>
       </c>
       <c r="D37" s="14"/>
-      <c r="E37" s="32"/>
+      <c r="E37" s="38"/>
     </row>
     <row r="38" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
@@ -1212,7 +1215,7 @@
         <f>SUM(D39:D41)</f>
         <v>0</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="36" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1224,7 +1227,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="18"/>
-      <c r="E39" s="31"/>
+      <c r="E39" s="37"/>
     </row>
     <row r="40" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="17" t="s">
@@ -1234,7 +1237,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="18"/>
-      <c r="E40" s="31"/>
+      <c r="E40" s="37"/>
     </row>
     <row r="41" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="13" t="s">
@@ -1244,7 +1247,7 @@
         <v>3</v>
       </c>
       <c r="D41" s="14"/>
-      <c r="E41" s="32"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
@@ -1258,7 +1261,7 @@
         <f>SUM(D43:D46)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="30" t="s">
+      <c r="E42" s="36" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1270,7 +1273,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="18"/>
-      <c r="E43" s="31"/>
+      <c r="E43" s="37"/>
     </row>
     <row r="44" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="17" t="s">
@@ -1280,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="D44" s="18"/>
-      <c r="E44" s="31"/>
+      <c r="E44" s="37"/>
     </row>
     <row r="45" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="17" t="s">
@@ -1290,7 +1293,7 @@
         <v>2</v>
       </c>
       <c r="D45" s="18"/>
-      <c r="E45" s="31"/>
+      <c r="E45" s="37"/>
     </row>
     <row r="46" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="13" t="s">
@@ -1300,7 +1303,7 @@
         <v>2</v>
       </c>
       <c r="D46" s="14"/>
-      <c r="E46" s="32"/>
+      <c r="E46" s="38"/>
     </row>
     <row r="47" spans="1:5" s="21" customFormat="1" ht="8.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:5" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
@@ -1310,11 +1313,11 @@
       <c r="B48" s="26"/>
       <c r="C48" s="6">
         <f>SUM(C2:C5,C9,C12:C17,C21:C23,C27:C29,C33,C35,C38,C42)</f>
-        <v>64.5</v>
+        <v>63.5</v>
       </c>
       <c r="D48" s="3">
         <f>SUM(D2:D5,D9,D12:D17,D21:D23,D27:D29,D33,D35,D38,D42)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Setting Up Gun Code
</commit_message>
<xml_diff>
--- a/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
+++ b/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Projects\2D-Mobile-Game\2D Mobile Game-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CADEF4-F8D1-419F-89FE-60E9C49DEF8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5497B85C-546E-4255-8392-3849A95F008A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
     <t>WORK IN PROGRESS</t>
   </si>
   <si>
-    <t>Create the code for gun pickup</t>
+    <t>Gun Code Broken</t>
   </si>
 </sst>
 </file>
@@ -366,6 +366,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -410,10 +414,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,10 +711,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="1" t="s">
         <v>47</v>
       </c>
@@ -779,7 +779,7 @@
         <f>SUM(D6:D8)</f>
         <v>3</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="29" t="s">
         <v>50</v>
       </c>
     </row>
@@ -793,7 +793,7 @@
       <c r="D6" s="8">
         <v>1</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
@@ -805,7 +805,7 @@
       <c r="D7" s="8">
         <v>1</v>
       </c>
-      <c r="E7" s="28"/>
+      <c r="E7" s="30"/>
     </row>
     <row r="8" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
@@ -817,7 +817,7 @@
       <c r="D8" s="10">
         <v>1</v>
       </c>
-      <c r="E8" s="29"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -831,7 +831,7 @@
         <f>SUM(D10:D11)</f>
         <v>3</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="29" t="s">
         <v>50</v>
       </c>
     </row>
@@ -845,7 +845,7 @@
       <c r="D10" s="8">
         <v>1.5</v>
       </c>
-      <c r="E10" s="28"/>
+      <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
@@ -857,7 +857,7 @@
       <c r="D11" s="10">
         <v>1.5</v>
       </c>
-      <c r="E11" s="29"/>
+      <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
@@ -939,35 +939,35 @@
       </c>
       <c r="D17" s="5">
         <f>SUM(D18:D20)</f>
-        <v>4</v>
-      </c>
-      <c r="E17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="39" t="s">
+    <row r="18" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="40">
-        <v>1</v>
-      </c>
-      <c r="D18" s="40">
-        <v>1</v>
-      </c>
-      <c r="E18" s="31"/>
-    </row>
-    <row r="19" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="39" t="s">
+      <c r="C18" s="25">
+        <v>1</v>
+      </c>
+      <c r="D18" s="25">
+        <v>1</v>
+      </c>
+      <c r="E18" s="33"/>
+    </row>
+    <row r="19" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="40">
-        <v>2</v>
-      </c>
-      <c r="D19" s="40">
-        <v>1</v>
-      </c>
-      <c r="E19" s="31"/>
+      <c r="C19" s="25">
+        <v>2</v>
+      </c>
+      <c r="D19" s="25">
+        <v>1</v>
+      </c>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
@@ -977,9 +977,9 @@
         <v>2</v>
       </c>
       <c r="D20" s="14">
-        <v>2</v>
-      </c>
-      <c r="E20" s="32"/>
+        <v>4</v>
+      </c>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
@@ -1021,7 +1021,7 @@
         <f>SUM(D24:D26)</f>
         <v>5</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="35" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
       <c r="D24" s="8">
         <v>1</v>
       </c>
-      <c r="E24" s="34"/>
+      <c r="E24" s="36"/>
     </row>
     <row r="25" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
@@ -1047,7 +1047,7 @@
       <c r="D25" s="8">
         <v>3</v>
       </c>
-      <c r="E25" s="34"/>
+      <c r="E25" s="36"/>
     </row>
     <row r="26" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="s">
@@ -1059,7 +1059,7 @@
       <c r="D26" s="10">
         <v>1</v>
       </c>
-      <c r="E26" s="35"/>
+      <c r="E26" s="37"/>
     </row>
     <row r="27" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
@@ -1099,7 +1099,7 @@
         <f>SUM(D30:D32)</f>
         <v>2.5</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="29" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       <c r="D30" s="8">
         <v>1</v>
       </c>
-      <c r="E30" s="28"/>
+      <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
@@ -1125,7 +1125,7 @@
       <c r="D31" s="8">
         <v>1</v>
       </c>
-      <c r="E31" s="28"/>
+      <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="s">
@@ -1137,7 +1137,7 @@
       <c r="D32" s="10">
         <v>0.5</v>
       </c>
-      <c r="E32" s="29"/>
+      <c r="E32" s="31"/>
     </row>
     <row r="33" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
@@ -1151,7 +1151,7 @@
         <f>D34</f>
         <v>5</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="29" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1165,7 +1165,7 @@
       <c r="D34" s="10">
         <v>5</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="E34" s="31"/>
     </row>
     <row r="35" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
@@ -1179,7 +1179,7 @@
         <f>SUM(D36:D37)</f>
         <v>0</v>
       </c>
-      <c r="E35" s="36" t="s">
+      <c r="E35" s="38" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1191,7 +1191,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="18"/>
-      <c r="E36" s="37"/>
+      <c r="E36" s="39"/>
     </row>
     <row r="37" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="13" t="s">
@@ -1201,7 +1201,7 @@
         <v>2</v>
       </c>
       <c r="D37" s="14"/>
-      <c r="E37" s="38"/>
+      <c r="E37" s="40"/>
     </row>
     <row r="38" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
@@ -1215,7 +1215,7 @@
         <f>SUM(D39:D41)</f>
         <v>0</v>
       </c>
-      <c r="E38" s="36" t="s">
+      <c r="E38" s="38" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="18"/>
-      <c r="E39" s="37"/>
+      <c r="E39" s="39"/>
     </row>
     <row r="40" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="17" t="s">
@@ -1237,7 +1237,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="18"/>
-      <c r="E40" s="37"/>
+      <c r="E40" s="39"/>
     </row>
     <row r="41" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="13" t="s">
@@ -1247,7 +1247,7 @@
         <v>3</v>
       </c>
       <c r="D41" s="14"/>
-      <c r="E41" s="38"/>
+      <c r="E41" s="40"/>
     </row>
     <row r="42" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
@@ -1261,7 +1261,7 @@
         <f>SUM(D43:D46)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="36" t="s">
+      <c r="E42" s="38" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1273,7 +1273,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="18"/>
-      <c r="E43" s="37"/>
+      <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="17" t="s">
@@ -1283,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="D44" s="18"/>
-      <c r="E44" s="37"/>
+      <c r="E44" s="39"/>
     </row>
     <row r="45" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="17" t="s">
@@ -1293,7 +1293,7 @@
         <v>2</v>
       </c>
       <c r="D45" s="18"/>
-      <c r="E45" s="37"/>
+      <c r="E45" s="39"/>
     </row>
     <row r="46" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="13" t="s">
@@ -1303,21 +1303,21 @@
         <v>2</v>
       </c>
       <c r="D46" s="14"/>
-      <c r="E46" s="38"/>
+      <c r="E46" s="40"/>
     </row>
     <row r="47" spans="1:5" s="21" customFormat="1" ht="8.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:5" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="26"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="6">
         <f>SUM(C2:C5,C9,C12:C17,C21:C23,C27:C29,C33,C35,C38,C42)</f>
         <v>63.5</v>
       </c>
       <c r="D48" s="3">
         <f>SUM(D2:D5,D9,D12:D17,D21:D23,D27:D29,D33,D35,D38,D42)</f>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Post processing Effects Done
</commit_message>
<xml_diff>
--- a/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
+++ b/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Projects\2D-Mobile-Game\2D Mobile Game-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD659557-E6AB-4241-911A-9A3EBA5E4815}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7DA8DC-6907-4D83-B169-2F81FA2F5F0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -690,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:E37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1160,41 +1160,45 @@
       </c>
       <c r="E34" s="28"/>
     </row>
-    <row r="35" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="7">
         <f>SUM(C36:C37)</f>
         <v>4</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="7">
         <f>SUM(D36:D37)</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="17">
-        <v>2</v>
-      </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="36"/>
-    </row>
-    <row r="37" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="12" t="s">
+      <c r="C36" s="7">
+        <v>2</v>
+      </c>
+      <c r="D36" s="7">
+        <v>4</v>
+      </c>
+      <c r="E36" s="27"/>
+    </row>
+    <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="13">
-        <v>2</v>
-      </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="37"/>
+      <c r="C37" s="9">
+        <v>2</v>
+      </c>
+      <c r="D37" s="9">
+        <v>2</v>
+      </c>
+      <c r="E37" s="28"/>
     </row>
     <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
@@ -1310,7 +1314,7 @@
       </c>
       <c r="D48" s="3">
         <f>SUM(D2:D5,D9,D12:D17,D21:D23,D27:D29,D33,D35,D38,D42)</f>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Particle Effects all set up and ready. Fixing Dash and Shift Effects
</commit_message>
<xml_diff>
--- a/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
+++ b/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Projects\2D-Mobile-Game\2D Mobile Game-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7DA8DC-6907-4D83-B169-2F81FA2F5F0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81EB4AB-C869-40EF-99E3-9EACB4D5E0A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Requirements</t>
   </si>
@@ -152,12 +152,6 @@
     <t>Particle Effects</t>
   </si>
   <si>
-    <t>Dash flames</t>
-  </si>
-  <si>
-    <t>Shift wind.</t>
-  </si>
-  <si>
     <t>Sparks for gravity pool</t>
   </si>
   <si>
@@ -195,6 +189,15 @@
   </si>
   <si>
     <t>Almost Done</t>
+  </si>
+  <si>
+    <t>Dash Sprites behind Trail</t>
+  </si>
+  <si>
+    <t>Shift gust of wind trail</t>
+  </si>
+  <si>
+    <t>Dash and Shift Particles set up but not showing</t>
   </si>
 </sst>
 </file>
@@ -690,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,10 +712,10 @@
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -729,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -743,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -757,7 +760,7 @@
         <v>2.5</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -773,7 +776,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -825,7 +828,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -863,7 +866,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -877,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -891,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -905,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -919,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -935,7 +938,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -985,7 +988,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -999,7 +1002,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -1015,7 +1018,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1063,7 +1066,7 @@
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1077,7 +1080,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -1093,7 +1096,7 @@
         <v>2.5</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1145,7 +1148,7 @@
         <v>5</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -1173,7 +1176,7 @@
         <v>6</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1210,45 +1213,51 @@
       </c>
       <c r="D38" s="15">
         <f>SUM(D39:D41)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E38" s="35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="7">
+        <v>2</v>
+      </c>
+      <c r="D39" s="7">
+        <v>2</v>
+      </c>
+      <c r="E39" s="36"/>
+    </row>
+    <row r="40" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="7">
+        <v>2</v>
+      </c>
+      <c r="D40" s="7">
+        <v>2</v>
+      </c>
+      <c r="E40" s="36"/>
+    </row>
+    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="17">
-        <v>2</v>
-      </c>
-      <c r="D39" s="17"/>
-      <c r="E39" s="36"/>
-    </row>
-    <row r="40" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="17">
-        <v>2</v>
-      </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="36"/>
-    </row>
-    <row r="41" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="13">
+      <c r="C41" s="9">
         <v>3</v>
       </c>
-      <c r="D41" s="13"/>
+      <c r="D41" s="9">
+        <v>2</v>
+      </c>
       <c r="E41" s="37"/>
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C42" s="15">
         <f>SUM(C43:C46)</f>
@@ -1259,12 +1268,12 @@
         <v>0</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C43" s="17">
         <v>2</v>
@@ -1274,7 +1283,7 @@
     </row>
     <row r="44" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C44" s="17">
         <v>2</v>
@@ -1284,7 +1293,7 @@
     </row>
     <row r="45" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C45" s="17">
         <v>2</v>
@@ -1294,7 +1303,7 @@
     </row>
     <row r="46" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C46" s="13">
         <v>2</v>
@@ -1305,7 +1314,7 @@
     <row r="47" spans="1:5" s="18" customFormat="1" ht="8.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:5" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A48" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48" s="25"/>
       <c r="C48" s="5">
@@ -1314,10 +1323,10 @@
       </c>
       <c r="D48" s="3">
         <f>SUM(D2:D5,D9,D12:D17,D21:D23,D27:D29,D33,D35,D38,D42)</f>
+        <v>56</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All Particles Working, Fixing Player Movement
</commit_message>
<xml_diff>
--- a/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
+++ b/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Projects\2D-Mobile-Game\2D Mobile Game-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81EB4AB-C869-40EF-99E3-9EACB4D5E0A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CA1875-39D3-4135-B22A-A1EC31B83FA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Requirements</t>
   </si>
@@ -188,23 +188,38 @@
     <t>WORK IN PROGRESS</t>
   </si>
   <si>
-    <t>Almost Done</t>
-  </si>
-  <si>
     <t>Dash Sprites behind Trail</t>
   </si>
   <si>
     <t>Shift gust of wind trail</t>
   </si>
   <si>
-    <t>Dash and Shift Particles set up but not showing</t>
+    <t>COMPLETELY STUCK ON THIS</t>
+  </si>
+  <si>
+    <t>EXTRAS</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>Volume Plugged in</t>
+  </si>
+  <si>
+    <t>Vibration Feedback</t>
+  </si>
+  <si>
+    <t>Publishing</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +259,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -277,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -314,11 +345,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -411,6 +508,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E46"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,16 +1176,16 @@
       </c>
       <c r="E26" s="34"/>
     </row>
-    <row r="27" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="38">
         <v>3</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="10" t="s">
-        <v>51</v>
+      <c r="D27" s="38"/>
+      <c r="E27" s="39" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1203,37 +1322,37 @@
       </c>
       <c r="E37" s="28"/>
     </row>
-    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14" t="s">
+    <row r="38" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="20">
         <f>SUM(C39:C41)</f>
         <v>7</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="20">
         <f>SUM(D39:D41)</f>
-        <v>6</v>
-      </c>
-      <c r="E38" s="35" t="s">
-        <v>54</v>
+        <v>7</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" s="7">
         <v>2</v>
       </c>
       <c r="D39" s="7">
-        <v>2</v>
-      </c>
-      <c r="E39" s="36"/>
+        <v>3</v>
+      </c>
+      <c r="E39" s="27"/>
     </row>
     <row r="40" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" s="7">
         <v>2</v>
@@ -1241,7 +1360,7 @@
       <c r="D40" s="7">
         <v>2</v>
       </c>
-      <c r="E40" s="36"/>
+      <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
@@ -1253,7 +1372,7 @@
       <c r="D41" s="9">
         <v>2</v>
       </c>
-      <c r="E41" s="37"/>
+      <c r="E41" s="28"/>
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
@@ -1323,14 +1442,57 @@
       </c>
       <c r="D48" s="3">
         <f>SUM(D2:D5,D9,D12:D17,D21:D23,D27:D29,D33,D35,D38,D42)</f>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>50</v>
       </c>
     </row>
+    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="A51" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="49"/>
+      <c r="C51" s="43"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="50"/>
+      <c r="C52" s="45"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="40"/>
+      <c r="B53" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="41"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="40"/>
+      <c r="B54" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" s="41"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="51"/>
+      <c r="C55" s="47"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="51"/>
+      <c r="C56" s="47"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A51:C51"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="E5:E8"/>

</xml_diff>

<commit_message>
Game prepped to just add sound
</commit_message>
<xml_diff>
--- a/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
+++ b/2D Mobile Game-Documentation/Gravity Boii Runner-Estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Projects\2D-Mobile-Game\2D Mobile Game-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CA1875-39D3-4135-B22A-A1EC31B83FA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CA5154-DB6D-4255-9E44-F360A724715E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,9 +194,6 @@
     <t>Shift gust of wind trail</t>
   </si>
   <si>
-    <t>COMPLETELY STUCK ON THIS</t>
-  </si>
-  <si>
     <t>EXTRAS</t>
   </si>
   <si>
@@ -213,13 +210,16 @@
   </si>
   <si>
     <t>Tutorial</t>
+  </si>
+  <si>
+    <t>Look into gunshot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,16 +261,21 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -415,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -463,6 +468,22 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -508,28 +529,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,10 +829,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
@@ -894,7 +897,7 @@
         <f>SUM(D6:D8)</f>
         <v>3</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="34" t="s">
         <v>48</v>
       </c>
     </row>
@@ -908,7 +911,7 @@
       <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="27"/>
+      <c r="E6" s="35"/>
     </row>
     <row r="7" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
@@ -920,7 +923,7 @@
       <c r="D7" s="7">
         <v>1</v>
       </c>
-      <c r="E7" s="27"/>
+      <c r="E7" s="35"/>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
@@ -932,7 +935,7 @@
       <c r="D8" s="9">
         <v>1</v>
       </c>
-      <c r="E8" s="28"/>
+      <c r="E8" s="36"/>
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -946,7 +949,7 @@
         <f>SUM(D10:D11)</f>
         <v>3</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="34" t="s">
         <v>48</v>
       </c>
     </row>
@@ -960,7 +963,7 @@
       <c r="D10" s="7">
         <v>1.5</v>
       </c>
-      <c r="E10" s="27"/>
+      <c r="E10" s="35"/>
     </row>
     <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
@@ -972,7 +975,7 @@
       <c r="D11" s="9">
         <v>1.5</v>
       </c>
-      <c r="E11" s="28"/>
+      <c r="E11" s="36"/>
     </row>
     <row r="12" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
@@ -1056,7 +1059,7 @@
         <f>SUM(D18:D20)</f>
         <v>7</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="37" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1070,7 +1073,7 @@
       <c r="D18" s="22">
         <v>1</v>
       </c>
-      <c r="E18" s="30"/>
+      <c r="E18" s="38"/>
     </row>
     <row r="19" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="21" t="s">
@@ -1082,7 +1085,7 @@
       <c r="D19" s="22">
         <v>1</v>
       </c>
-      <c r="E19" s="30"/>
+      <c r="E19" s="38"/>
     </row>
     <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
@@ -1094,7 +1097,7 @@
       <c r="D20" s="9">
         <v>5</v>
       </c>
-      <c r="E20" s="31"/>
+      <c r="E20" s="39"/>
     </row>
     <row r="21" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
@@ -1136,7 +1139,7 @@
         <f>SUM(D24:D26)</f>
         <v>5</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="40" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1150,7 +1153,7 @@
       <c r="D24" s="7">
         <v>1</v>
       </c>
-      <c r="E24" s="33"/>
+      <c r="E24" s="41"/>
     </row>
     <row r="25" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
@@ -1162,7 +1165,7 @@
       <c r="D25" s="7">
         <v>3</v>
       </c>
-      <c r="E25" s="33"/>
+      <c r="E25" s="41"/>
     </row>
     <row r="26" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
@@ -1174,18 +1177,20 @@
       <c r="D26" s="9">
         <v>1</v>
       </c>
-      <c r="E26" s="34"/>
-    </row>
-    <row r="27" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="39" t="s">
+      <c r="E26" s="42"/>
+    </row>
+    <row r="27" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="38">
+      <c r="C27" s="26">
         <v>3</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="39" t="s">
-        <v>53</v>
+      <c r="D27" s="26">
+        <v>6</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1214,8 +1219,8 @@
         <f>SUM(D30:D32)</f>
         <v>2.5</v>
       </c>
-      <c r="E29" s="26" t="s">
-        <v>48</v>
+      <c r="E29" s="34" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1228,7 +1233,7 @@
       <c r="D30" s="7">
         <v>1</v>
       </c>
-      <c r="E30" s="27"/>
+      <c r="E30" s="35"/>
     </row>
     <row r="31" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
@@ -1240,7 +1245,7 @@
       <c r="D31" s="7">
         <v>1</v>
       </c>
-      <c r="E31" s="27"/>
+      <c r="E31" s="35"/>
     </row>
     <row r="32" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
@@ -1252,7 +1257,7 @@
       <c r="D32" s="9">
         <v>0.5</v>
       </c>
-      <c r="E32" s="28"/>
+      <c r="E32" s="36"/>
     </row>
     <row r="33" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
@@ -1266,7 +1271,7 @@
         <f>D34</f>
         <v>5</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="34" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1280,7 +1285,7 @@
       <c r="D34" s="9">
         <v>5</v>
       </c>
-      <c r="E34" s="28"/>
+      <c r="E34" s="36"/>
     </row>
     <row r="35" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
@@ -1294,7 +1299,7 @@
         <f>SUM(D36:D37)</f>
         <v>6</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E35" s="34" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1308,7 +1313,7 @@
       <c r="D36" s="7">
         <v>4</v>
       </c>
-      <c r="E36" s="27"/>
+      <c r="E36" s="35"/>
     </row>
     <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
@@ -1320,7 +1325,7 @@
       <c r="D37" s="9">
         <v>2</v>
       </c>
-      <c r="E37" s="28"/>
+      <c r="E37" s="36"/>
     </row>
     <row r="38" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
@@ -1334,7 +1339,7 @@
         <f>SUM(D39:D41)</f>
         <v>7</v>
       </c>
-      <c r="E38" s="26" t="s">
+      <c r="E38" s="34" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1348,7 +1353,7 @@
       <c r="D39" s="7">
         <v>3</v>
       </c>
-      <c r="E39" s="27"/>
+      <c r="E39" s="35"/>
     </row>
     <row r="40" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="6" t="s">
@@ -1360,7 +1365,7 @@
       <c r="D40" s="7">
         <v>2</v>
       </c>
-      <c r="E40" s="27"/>
+      <c r="E40" s="35"/>
     </row>
     <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
@@ -1372,7 +1377,7 @@
       <c r="D41" s="9">
         <v>2</v>
       </c>
-      <c r="E41" s="28"/>
+      <c r="E41" s="36"/>
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
@@ -1386,7 +1391,7 @@
         <f>SUM(D43:D46)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="43" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1398,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="17"/>
-      <c r="E43" s="36"/>
+      <c r="E43" s="44"/>
     </row>
     <row r="44" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="16" t="s">
@@ -1408,7 +1413,7 @@
         <v>2</v>
       </c>
       <c r="D44" s="17"/>
-      <c r="E44" s="36"/>
+      <c r="E44" s="44"/>
     </row>
     <row r="45" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="16" t="s">
@@ -1418,7 +1423,7 @@
         <v>2</v>
       </c>
       <c r="D45" s="17"/>
-      <c r="E45" s="36"/>
+      <c r="E45" s="44"/>
     </row>
     <row r="46" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="12" t="s">
@@ -1428,67 +1433,67 @@
         <v>2</v>
       </c>
       <c r="D46" s="13"/>
-      <c r="E46" s="37"/>
+      <c r="E46" s="45"/>
     </row>
     <row r="47" spans="1:5" s="18" customFormat="1" ht="8.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:5" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="25"/>
+      <c r="B48" s="33"/>
       <c r="C48" s="5">
         <f>SUM(C2:C5,C9,C12:C17,C21:C23,C27:C29,C33,C35,C38,C42)</f>
         <v>63.5</v>
       </c>
       <c r="D48" s="3">
         <f>SUM(D2:D5,D9,D12:D17,D21:D23,D27:D29,D33,D35,D38,D42)</f>
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A51" s="42" t="s">
+      <c r="A51" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="29"/>
+      <c r="C51" s="30"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="49"/>
-      <c r="C51" s="43"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="44" t="s">
+      <c r="B52" s="19"/>
+      <c r="C52" s="47"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="48"/>
+      <c r="B53" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="50"/>
-      <c r="C52" s="45"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="40"/>
-      <c r="B53" s="48" t="s">
+      <c r="C53" s="49"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="48"/>
+      <c r="B54" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="41"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="40"/>
-      <c r="B54" s="48" t="s">
+      <c r="C54" s="49"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="41"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="46" t="s">
+      <c r="B55" s="25"/>
+      <c r="C55" s="24"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="51"/>
-      <c r="C55" s="47"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" s="51"/>
-      <c r="C56" s="47"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>